<commit_message>
Aggregate together simple network analysis
</commit_message>
<xml_diff>
--- a/analysis_complex-network_tdma.xlsx
+++ b/analysis_complex-network_tdma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weiff\Desktop\everything\projects\NetworkSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49E2AE0-93A8-4393-9EFF-78898ACF8193}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA78247A-BB1A-4878-9660-4A8A3BC94F04}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0.1" sheetId="3" r:id="rId1"/>
@@ -61,9 +61,6 @@
     <t>"33333333333333333333"</t>
   </si>
   <si>
-    <t>Polling</t>
-  </si>
-  <si>
     <t>Messages Sent</t>
   </si>
   <si>
@@ -77,6 +74,9 @@
   </si>
   <si>
     <t>Message Ratio</t>
+  </si>
+  <si>
+    <t>TDMA</t>
   </si>
 </sst>
 </file>
@@ -2750,9 +2750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2761,19 +2759,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -2967,7 +2965,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>

</xml_diff>